<commit_message>
Changes to GUI EventLog
</commit_message>
<xml_diff>
--- a/01CommonDataForBattery/z_BalancerCurrentMeasurement.xlsx
+++ b/01CommonDataForBattery/z_BalancerCurrentMeasurement.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20367"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20368"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\School Related\Masters\00-Grad_Research\Projects\00BattManager\03DataGen\01CommonDataForBattery\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E13DAE23-5C30-4F61-935E-CE8F0ACD0E6D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91C57923-58E4-4D03-BCF3-CFFAF912D181}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="6" activeTab="8" xr2:uid="{7F21F5D0-71D5-4345-AB2F-02B2A07085A9}"/>
   </bookViews>
@@ -646,13 +646,13 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -669,6 +669,2075 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'4-Cell Config Rnd5_B4_RTON_chg'!$M$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'4-Cell Config Rnd5_B4_RTON_chg'!$M$2:$M$53</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="52"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-0.25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-0.34</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-0.44</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-0.44</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-0.44</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-0.28999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-0.34</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-0.2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-0.25</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-0.49</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-0.39</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-0.34</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-0.28999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-0.34</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-0.34</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-0.34</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>-0.44</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>-0.34</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>-0.34</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>-0.44</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>-0.34</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>-0.44</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>-0.44</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>-0.39</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>-0.34</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>-0.44</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>-0.28999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>-0.28999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>-0.34</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>-0.28999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>-0.44</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>-0.34</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>-0.39</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>-0.28999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>-0.28999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>-0.44</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>-0.34</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>-0.28999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>-0.34</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>-0.39</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>-0.39</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>-0.39</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>-0.49</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>-0.28999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>-0.34</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>-0.44</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>-0.28999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>-0.39</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>-0.34</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>-0.2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-1F60-4BE9-BD6B-4AF8EDAFF9AF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1874666048"/>
+        <c:axId val="1747416448"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1874666048"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1747416448"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1747416448"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1874666048"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'4-Cell Config Rnd5_B4_RTON_chg'!$N$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'4-Cell Config Rnd5_B4_RTON_chg'!$N$2:$N$53</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="52"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.15</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-0.05</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-0.05</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.15</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.15</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.15</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>-0.1</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.15</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.15</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.15</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>-0.05</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0.15</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4B9E-439F-AF28-796D048F66AB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1737092752"/>
+        <c:axId val="1746617856"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1737092752"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1746617856"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1746617856"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1737092752"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>129540</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>129540</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2E189DB1-A8E2-4BAE-B41C-3C343CC4005B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>358140</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AA123BB6-CADC-4818-A9CE-36FB0B789404}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -20543,42 +22612,42 @@
       <c r="E1" s="51"/>
       <c r="F1" s="51"/>
       <c r="G1" s="51"/>
-      <c r="J1" s="64" t="s">
+      <c r="J1" s="62" t="s">
         <v>43</v>
       </c>
-      <c r="K1" s="64"/>
-      <c r="L1" s="64"/>
-      <c r="M1" s="64"/>
-      <c r="N1" s="64"/>
-      <c r="O1" s="64"/>
-      <c r="P1" s="64"/>
-      <c r="S1" s="64" t="s">
+      <c r="K1" s="62"/>
+      <c r="L1" s="62"/>
+      <c r="M1" s="62"/>
+      <c r="N1" s="62"/>
+      <c r="O1" s="62"/>
+      <c r="P1" s="62"/>
+      <c r="S1" s="62" t="s">
         <v>43</v>
       </c>
-      <c r="T1" s="64"/>
-      <c r="U1" s="64"/>
-      <c r="V1" s="64"/>
-      <c r="W1" s="64"/>
-      <c r="X1" s="64"/>
-      <c r="Y1" s="64"/>
-      <c r="AB1" s="64" t="s">
+      <c r="T1" s="62"/>
+      <c r="U1" s="62"/>
+      <c r="V1" s="62"/>
+      <c r="W1" s="62"/>
+      <c r="X1" s="62"/>
+      <c r="Y1" s="62"/>
+      <c r="AB1" s="62" t="s">
         <v>44</v>
       </c>
-      <c r="AC1" s="64"/>
-      <c r="AD1" s="64"/>
-      <c r="AE1" s="64"/>
-      <c r="AF1" s="64"/>
-      <c r="AG1" s="64"/>
-      <c r="AH1" s="64"/>
-      <c r="AK1" s="64" t="s">
+      <c r="AC1" s="62"/>
+      <c r="AD1" s="62"/>
+      <c r="AE1" s="62"/>
+      <c r="AF1" s="62"/>
+      <c r="AG1" s="62"/>
+      <c r="AH1" s="62"/>
+      <c r="AK1" s="62" t="s">
         <v>44</v>
       </c>
-      <c r="AL1" s="64"/>
-      <c r="AM1" s="64"/>
-      <c r="AN1" s="64"/>
-      <c r="AO1" s="64"/>
-      <c r="AP1" s="64"/>
-      <c r="AQ1" s="64"/>
+      <c r="AL1" s="62"/>
+      <c r="AM1" s="62"/>
+      <c r="AN1" s="62"/>
+      <c r="AO1" s="62"/>
+      <c r="AP1" s="62"/>
+      <c r="AQ1" s="62"/>
     </row>
     <row r="2" spans="1:43" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="46" t="s">
@@ -21295,8 +23364,8 @@
       <c r="G10" s="1">
         <v>0.1</v>
       </c>
-      <c r="J10" s="62"/>
-      <c r="K10" s="62"/>
+      <c r="J10" s="64"/>
+      <c r="K10" s="64"/>
       <c r="N10" s="1">
         <v>-0.59</v>
       </c>
@@ -21306,8 +23375,8 @@
       <c r="P10" s="1">
         <v>0</v>
       </c>
-      <c r="S10" s="62"/>
-      <c r="T10" s="62"/>
+      <c r="S10" s="64"/>
+      <c r="T10" s="64"/>
       <c r="W10" s="1">
         <v>0.39</v>
       </c>
@@ -21317,8 +23386,8 @@
       <c r="Y10" s="1">
         <v>0.05</v>
       </c>
-      <c r="AB10" s="62"/>
-      <c r="AC10" s="62"/>
+      <c r="AB10" s="64"/>
+      <c r="AC10" s="64"/>
       <c r="AD10" s="26"/>
       <c r="AE10" s="1"/>
       <c r="AF10" s="1">
@@ -21330,8 +23399,8 @@
       <c r="AH10" s="1">
         <v>0.1</v>
       </c>
-      <c r="AK10" s="62"/>
-      <c r="AL10" s="62"/>
+      <c r="AK10" s="64"/>
+      <c r="AL10" s="64"/>
       <c r="AM10" s="26"/>
       <c r="AN10" s="1"/>
       <c r="AO10" s="1">
@@ -21433,8 +23502,8 @@
       <c r="G12" s="1">
         <v>0.1</v>
       </c>
-      <c r="J12" s="62"/>
-      <c r="K12" s="62"/>
+      <c r="J12" s="64"/>
+      <c r="K12" s="64"/>
       <c r="N12" s="1">
         <v>-0.88</v>
       </c>
@@ -21444,8 +23513,8 @@
       <c r="P12" s="1">
         <v>0.25</v>
       </c>
-      <c r="S12" s="62"/>
-      <c r="T12" s="62"/>
+      <c r="S12" s="64"/>
+      <c r="T12" s="64"/>
       <c r="W12" s="1">
         <v>0.49</v>
       </c>
@@ -21455,8 +23524,8 @@
       <c r="Y12" s="1">
         <v>0.1</v>
       </c>
-      <c r="AB12" s="62"/>
-      <c r="AC12" s="62"/>
+      <c r="AB12" s="64"/>
+      <c r="AC12" s="64"/>
       <c r="AD12" s="26"/>
       <c r="AE12" s="1"/>
       <c r="AF12" s="1">
@@ -21468,8 +23537,8 @@
       <c r="AH12" s="1">
         <v>0.15</v>
       </c>
-      <c r="AK12" s="62"/>
-      <c r="AL12" s="62"/>
+      <c r="AK12" s="64"/>
+      <c r="AL12" s="64"/>
       <c r="AM12" s="26"/>
       <c r="AN12" s="1"/>
       <c r="AO12" s="1">
@@ -23453,13 +25522,20 @@
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="AB2:AH2"/>
-    <mergeCell ref="AK2:AQ2"/>
-    <mergeCell ref="J1:P1"/>
-    <mergeCell ref="S1:Y1"/>
-    <mergeCell ref="AB1:AH1"/>
-    <mergeCell ref="AK1:AQ1"/>
-    <mergeCell ref="S2:Y2"/>
+    <mergeCell ref="S9:U9"/>
+    <mergeCell ref="S11:U11"/>
+    <mergeCell ref="S13:U13"/>
+    <mergeCell ref="AK12:AL12"/>
+    <mergeCell ref="AB9:AD9"/>
+    <mergeCell ref="AK9:AM9"/>
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="J13:L13"/>
+    <mergeCell ref="J11:L11"/>
+    <mergeCell ref="J9:L9"/>
+    <mergeCell ref="J2:P2"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="J12:K12"/>
     <mergeCell ref="AK14:AL14"/>
     <mergeCell ref="AB10:AC10"/>
     <mergeCell ref="AB12:AC12"/>
@@ -23472,20 +25548,13 @@
     <mergeCell ref="AB13:AD13"/>
     <mergeCell ref="AK11:AM11"/>
     <mergeCell ref="AK13:AM13"/>
-    <mergeCell ref="A2:G2"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="J13:L13"/>
-    <mergeCell ref="J11:L11"/>
-    <mergeCell ref="J9:L9"/>
-    <mergeCell ref="J2:P2"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="J12:K12"/>
-    <mergeCell ref="S9:U9"/>
-    <mergeCell ref="S11:U11"/>
-    <mergeCell ref="S13:U13"/>
-    <mergeCell ref="AK12:AL12"/>
-    <mergeCell ref="AB9:AD9"/>
-    <mergeCell ref="AK9:AM9"/>
+    <mergeCell ref="AB2:AH2"/>
+    <mergeCell ref="AK2:AQ2"/>
+    <mergeCell ref="J1:P1"/>
+    <mergeCell ref="S1:Y1"/>
+    <mergeCell ref="AB1:AH1"/>
+    <mergeCell ref="AK1:AQ1"/>
+    <mergeCell ref="S2:Y2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -33655,11 +35724,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="BV10:BX10"/>
-    <mergeCell ref="BV18:BX18"/>
-    <mergeCell ref="AW1:BC1"/>
-    <mergeCell ref="BE1:BK1"/>
-    <mergeCell ref="BN1:BT1"/>
     <mergeCell ref="AP11:AR11"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="I1:O1"/>
@@ -33667,6 +35731,11 @@
     <mergeCell ref="Y1:AE1"/>
     <mergeCell ref="AG1:AM1"/>
     <mergeCell ref="AO1:AU1"/>
+    <mergeCell ref="BV10:BX10"/>
+    <mergeCell ref="BV18:BX18"/>
+    <mergeCell ref="AW1:BC1"/>
+    <mergeCell ref="BE1:BK1"/>
+    <mergeCell ref="BN1:BT1"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -33695,51 +35764,51 @@
       <c r="E1" s="51"/>
       <c r="F1" s="51"/>
       <c r="G1" s="51"/>
-      <c r="I1" s="64" t="s">
+      <c r="I1" s="62" t="s">
         <v>49</v>
       </c>
-      <c r="J1" s="64"/>
-      <c r="K1" s="64"/>
-      <c r="L1" s="64"/>
-      <c r="M1" s="64"/>
-      <c r="N1" s="64"/>
-      <c r="O1" s="64"/>
-      <c r="R1" s="64" t="s">
+      <c r="J1" s="62"/>
+      <c r="K1" s="62"/>
+      <c r="L1" s="62"/>
+      <c r="M1" s="62"/>
+      <c r="N1" s="62"/>
+      <c r="O1" s="62"/>
+      <c r="R1" s="62" t="s">
         <v>49</v>
       </c>
-      <c r="S1" s="64"/>
-      <c r="T1" s="64"/>
-      <c r="U1" s="64"/>
-      <c r="V1" s="64"/>
-      <c r="W1" s="64"/>
-      <c r="X1" s="64"/>
-      <c r="AA1" s="64" t="s">
+      <c r="S1" s="62"/>
+      <c r="T1" s="62"/>
+      <c r="U1" s="62"/>
+      <c r="V1" s="62"/>
+      <c r="W1" s="62"/>
+      <c r="X1" s="62"/>
+      <c r="AA1" s="62" t="s">
         <v>49</v>
       </c>
-      <c r="AB1" s="64"/>
-      <c r="AC1" s="64"/>
-      <c r="AD1" s="64"/>
-      <c r="AE1" s="64"/>
-      <c r="AF1" s="64"/>
-      <c r="AG1" s="64"/>
-      <c r="AJ1" s="64" t="s">
+      <c r="AB1" s="62"/>
+      <c r="AC1" s="62"/>
+      <c r="AD1" s="62"/>
+      <c r="AE1" s="62"/>
+      <c r="AF1" s="62"/>
+      <c r="AG1" s="62"/>
+      <c r="AJ1" s="62" t="s">
         <v>43</v>
       </c>
-      <c r="AK1" s="64"/>
-      <c r="AL1" s="64"/>
-      <c r="AM1" s="64"/>
-      <c r="AN1" s="64"/>
-      <c r="AO1" s="64"/>
-      <c r="AP1" s="64"/>
-      <c r="AS1" s="64" t="s">
+      <c r="AK1" s="62"/>
+      <c r="AL1" s="62"/>
+      <c r="AM1" s="62"/>
+      <c r="AN1" s="62"/>
+      <c r="AO1" s="62"/>
+      <c r="AP1" s="62"/>
+      <c r="AS1" s="62" t="s">
         <v>43</v>
       </c>
-      <c r="AT1" s="64"/>
-      <c r="AU1" s="64"/>
-      <c r="AV1" s="64"/>
-      <c r="AW1" s="64"/>
-      <c r="AX1" s="64"/>
-      <c r="AY1" s="64"/>
+      <c r="AT1" s="62"/>
+      <c r="AU1" s="62"/>
+      <c r="AV1" s="62"/>
+      <c r="AW1" s="62"/>
+      <c r="AX1" s="62"/>
+      <c r="AY1" s="62"/>
     </row>
     <row r="2" spans="1:51" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="46" t="s">
@@ -34478,8 +36547,8 @@
       <c r="G10" s="30">
         <v>0.1</v>
       </c>
-      <c r="I10" s="62"/>
-      <c r="J10" s="62"/>
+      <c r="I10" s="64"/>
+      <c r="J10" s="64"/>
       <c r="M10" s="30">
         <v>-0.1</v>
       </c>
@@ -34489,8 +36558,8 @@
       <c r="O10" s="30">
         <v>1.86</v>
       </c>
-      <c r="R10" s="62"/>
-      <c r="S10" s="62"/>
+      <c r="R10" s="64"/>
+      <c r="S10" s="64"/>
       <c r="V10" s="30">
         <v>-0.05</v>
       </c>
@@ -34500,8 +36569,8 @@
       <c r="X10" s="30">
         <v>-0.05</v>
       </c>
-      <c r="AA10" s="62"/>
-      <c r="AB10" s="62"/>
+      <c r="AA10" s="64"/>
+      <c r="AB10" s="64"/>
       <c r="AE10" s="30">
         <v>0.24</v>
       </c>
@@ -34511,10 +36580,10 @@
       <c r="AG10" s="30">
         <v>-0.05</v>
       </c>
-      <c r="AJ10" s="62"/>
-      <c r="AK10" s="62"/>
-      <c r="AS10" s="62"/>
-      <c r="AT10" s="62"/>
+      <c r="AJ10" s="64"/>
+      <c r="AK10" s="64"/>
+      <c r="AS10" s="64"/>
+      <c r="AT10" s="64"/>
     </row>
     <row r="11" spans="1:51" x14ac:dyDescent="0.3">
       <c r="E11" s="30">
@@ -34604,8 +36673,8 @@
       <c r="G12" s="30">
         <v>0.1</v>
       </c>
-      <c r="I12" s="62"/>
-      <c r="J12" s="62"/>
+      <c r="I12" s="64"/>
+      <c r="J12" s="64"/>
       <c r="M12" s="30">
         <v>-0.15</v>
       </c>
@@ -34615,8 +36684,8 @@
       <c r="O12" s="30">
         <v>1.86</v>
       </c>
-      <c r="R12" s="62"/>
-      <c r="S12" s="62"/>
+      <c r="R12" s="64"/>
+      <c r="S12" s="64"/>
       <c r="V12" s="30">
         <v>-0.2</v>
       </c>
@@ -34626,8 +36695,8 @@
       <c r="X12" s="30">
         <v>0</v>
       </c>
-      <c r="AA12" s="62"/>
-      <c r="AB12" s="62"/>
+      <c r="AA12" s="64"/>
+      <c r="AB12" s="64"/>
       <c r="AE12" s="30">
         <v>0.28999999999999998</v>
       </c>
@@ -34637,10 +36706,10 @@
       <c r="AG12" s="30">
         <v>-0.05</v>
       </c>
-      <c r="AJ12" s="62"/>
-      <c r="AK12" s="62"/>
-      <c r="AS12" s="62"/>
-      <c r="AT12" s="62"/>
+      <c r="AJ12" s="64"/>
+      <c r="AK12" s="64"/>
+      <c r="AS12" s="64"/>
+      <c r="AT12" s="64"/>
     </row>
     <row r="13" spans="1:51" x14ac:dyDescent="0.3">
       <c r="E13" s="30">
@@ -36274,16 +38343,28 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="A2:G2"/>
-    <mergeCell ref="R2:X2"/>
-    <mergeCell ref="AA2:AG2"/>
-    <mergeCell ref="AJ2:AP2"/>
-    <mergeCell ref="AS2:AY2"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="R1:X1"/>
-    <mergeCell ref="AA1:AG1"/>
-    <mergeCell ref="AJ1:AP1"/>
-    <mergeCell ref="AS1:AY1"/>
+    <mergeCell ref="I13:K13"/>
+    <mergeCell ref="I1:O1"/>
+    <mergeCell ref="I2:O2"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="I11:K11"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="R13:T13"/>
+    <mergeCell ref="AA13:AC13"/>
+    <mergeCell ref="AJ13:AL13"/>
+    <mergeCell ref="AS13:AU13"/>
+    <mergeCell ref="AA14:AB14"/>
+    <mergeCell ref="AJ14:AK14"/>
+    <mergeCell ref="AS14:AT14"/>
+    <mergeCell ref="R11:T11"/>
+    <mergeCell ref="AA11:AC11"/>
+    <mergeCell ref="AJ11:AL11"/>
+    <mergeCell ref="AS11:AU11"/>
+    <mergeCell ref="R12:S12"/>
+    <mergeCell ref="AA12:AB12"/>
+    <mergeCell ref="AJ12:AK12"/>
+    <mergeCell ref="AS12:AT12"/>
     <mergeCell ref="R9:T9"/>
     <mergeCell ref="AA9:AC9"/>
     <mergeCell ref="AJ9:AL9"/>
@@ -36292,28 +38373,16 @@
     <mergeCell ref="AA10:AB10"/>
     <mergeCell ref="AJ10:AK10"/>
     <mergeCell ref="AS10:AT10"/>
-    <mergeCell ref="R11:T11"/>
-    <mergeCell ref="AA11:AC11"/>
-    <mergeCell ref="AJ11:AL11"/>
-    <mergeCell ref="AS11:AU11"/>
-    <mergeCell ref="R12:S12"/>
-    <mergeCell ref="AA12:AB12"/>
-    <mergeCell ref="AJ12:AK12"/>
-    <mergeCell ref="AS12:AT12"/>
-    <mergeCell ref="R13:T13"/>
-    <mergeCell ref="AA13:AC13"/>
-    <mergeCell ref="AJ13:AL13"/>
-    <mergeCell ref="AS13:AU13"/>
-    <mergeCell ref="AA14:AB14"/>
-    <mergeCell ref="AJ14:AK14"/>
-    <mergeCell ref="AS14:AT14"/>
-    <mergeCell ref="I13:K13"/>
-    <mergeCell ref="I1:O1"/>
-    <mergeCell ref="I2:O2"/>
-    <mergeCell ref="I9:K9"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="I11:K11"/>
-    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="R1:X1"/>
+    <mergeCell ref="AA1:AG1"/>
+    <mergeCell ref="AJ1:AP1"/>
+    <mergeCell ref="AS1:AY1"/>
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="R2:X2"/>
+    <mergeCell ref="AA2:AG2"/>
+    <mergeCell ref="AJ2:AP2"/>
+    <mergeCell ref="AS2:AY2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -36324,7 +38393,7 @@
   <dimension ref="A1:BX53"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
+      <selection activeCell="N2" sqref="N1:N1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -37604,6 +39673,10 @@
       <c r="G16" s="35">
         <v>0.05</v>
       </c>
+      <c r="L16" s="35">
+        <f>L3+ABS(J3)</f>
+        <v>2.1628000000000007</v>
+      </c>
       <c r="M16" s="35">
         <v>-0.34</v>
       </c>
@@ -38775,19 +40848,20 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="AW1:BC1"/>
+    <mergeCell ref="BE1:BK1"/>
+    <mergeCell ref="BN1:BT1"/>
+    <mergeCell ref="BV10:BX10"/>
+    <mergeCell ref="BV18:BX18"/>
     <mergeCell ref="AO1:AU1"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="I1:O1"/>
     <mergeCell ref="Q1:W1"/>
     <mergeCell ref="Y1:AE1"/>
     <mergeCell ref="AG1:AM1"/>
-    <mergeCell ref="AW1:BC1"/>
-    <mergeCell ref="BE1:BK1"/>
-    <mergeCell ref="BN1:BT1"/>
-    <mergeCell ref="BV10:BX10"/>
-    <mergeCell ref="BV18:BX18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>